<commit_message>
change xsd create sample bugfix
</commit_message>
<xml_diff>
--- a/core/test/sample/incomes.xlsx
+++ b/core/test/sample/incomes.xlsx
@@ -24,12 +24,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Месяц</t>
-  </si>
-  <si>
-    <t>Выручка</t>
-  </si>
-  <si>
     <t>${month}</t>
   </si>
   <si>
@@ -37,6 +31,12 @@
   </si>
   <si>
     <t>Итого</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Income</t>
   </si>
 </sst>
 </file>
@@ -191,24 +191,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="66032000"/>
-        <c:axId val="66033536"/>
+        <c:axId val="55480704"/>
+        <c:axId val="55482240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66032000"/>
+        <c:axId val="55480704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66033536"/>
+        <c:crossAx val="55482240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66033536"/>
+        <c:axId val="55482240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -216,7 +216,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66032000"/>
+        <c:crossAx val="55480704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -229,7 +229,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -558,7 +558,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="A4:G17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -569,23 +569,23 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <f>SUM(B2:B2)</f>

</xml_diff>